<commit_message>
Instruction Modification, Add score shown system
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Localization.xlsx
+++ b/Assets/StreamingAssets/Localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elegetic\TellltheAuthority\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ECB228-31E4-4251-BC0D-21915FD3522D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB72FB46-B747-4267-9571-69B5AF7D5C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{C21F6677-7B9D-48C9-8722-1AB02A4EB084}"/>
+    <workbookView xWindow="3300" yWindow="1710" windowWidth="19200" windowHeight="11170" xr2:uid="{C21F6677-7B9D-48C9-8722-1AB02A4EB084}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="130">
   <si>
     <t>EN_GB</t>
   </si>
@@ -368,6 +368,66 @@
   </si>
   <si>
     <t>目标分数</t>
+  </si>
+  <si>
+    <t>REPORT STATUS</t>
+  </si>
+  <si>
+    <t>REPORT AUTHORITY</t>
+  </si>
+  <si>
+    <t>SCORE CHANGE</t>
+  </si>
+  <si>
+    <t>NOT CRIMINAL</t>
+  </si>
+  <si>
+    <t>CRIMINAL</t>
+  </si>
+  <si>
+    <t>WRONG</t>
+  </si>
+  <si>
+    <t>CORRECT</t>
+  </si>
+  <si>
+    <t>COMBO BONUS</t>
+  </si>
+  <si>
+    <t>连对加分</t>
+  </si>
+  <si>
+    <t>举报状态</t>
+  </si>
+  <si>
+    <t>举报机构</t>
+  </si>
+  <si>
+    <t>分数变化</t>
+  </si>
+  <si>
+    <t>未犯罪</t>
+  </si>
+  <si>
+    <t>犯罪</t>
+  </si>
+  <si>
+    <t>错误</t>
+  </si>
+  <si>
+    <t>正确</t>
+  </si>
+  <si>
+    <t>CURRENT SCORES</t>
+  </si>
+  <si>
+    <t>分数纪录</t>
+  </si>
+  <si>
+    <t>CURRENT TOTAL</t>
+  </si>
+  <si>
+    <t>当前总分</t>
   </si>
 </sst>
 </file>
@@ -745,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679472E8-4440-48DF-8D5D-1D03DFA57972}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1238,6 +1298,86 @@
         <v>109</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>